<commit_message>
Edited github folder generating code to match spreadsheet changes
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_FRAMEWORKS_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_FRAMEWORKS_MASTER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sara/Dropbox/SJT_Projects_current/AMITT/CODE_AND_DATA/github_cogseccollab_AMITT/AMITT_MASTER_DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C3D11D-79CE-0440-8B95-BB4A9A1F9532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A563B6-C24E-BB42-9014-A4E35A84CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5420" yWindow="-24700" windowWidth="37000" windowHeight="23920" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="-20500" windowWidth="37000" windowHeight="21100" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADMIN_README" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="1794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3185" uniqueCount="1811">
   <si>
     <t>MASTER COPY OF AMITT TTPS</t>
   </si>
@@ -7146,6 +7146,57 @@
   </si>
   <si>
     <t>Look at Ad trackers, Tracking ids, Tracking ads, Re-use of as features (language, name, themes, plug-in, re-use/versions)</t>
+  </si>
+  <si>
+    <t>name_DE</t>
+  </si>
+  <si>
+    <t>summary_DE</t>
+  </si>
+  <si>
+    <t>Planung</t>
+  </si>
+  <si>
+    <t>Vorbereitung</t>
+  </si>
+  <si>
+    <t>Durchführung</t>
+  </si>
+  <si>
+    <t>Auswertung</t>
+  </si>
+  <si>
+    <t>strategische Planung</t>
+  </si>
+  <si>
+    <t>objektive Planung</t>
+  </si>
+  <si>
+    <t>Menschen entwickeln</t>
+  </si>
+  <si>
+    <t>Netzwerke entwickeln</t>
+  </si>
+  <si>
+    <t>individualisierte Wählerwerbung</t>
+  </si>
+  <si>
+    <t>Inhalte entwickeln</t>
+  </si>
+  <si>
+    <t>Kanalauswahl</t>
+  </si>
+  <si>
+    <t>Ankurbelung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research intended audience.  Includes audience segmentation, hot-button issues etc. </t>
+  </si>
+  <si>
+    <t>Design the campaign(s) needed to meet the incident goals</t>
+  </si>
+  <si>
+    <t>Identify groups that can best be used to meet incident goals</t>
   </si>
 </sst>
 </file>
@@ -7458,7 +7509,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -7761,6 +7812,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8588,7 +8651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057EA134-8119-C141-96AC-8F3F758DF5E6}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -12220,23 +12283,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ10"/>
+  <dimension ref="A1:AML10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6" max="1024" width="16.33203125" style="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="54.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8" max="1026" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>1421</v>
       </c>
@@ -12244,121 +12308,153 @@
         <v>57</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
+        <v>1795</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="38.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="38.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="24" t="s">
+        <v>1796</v>
+      </c>
+      <c r="D2" s="20">
         <v>1</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="E2" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="30" t="str">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30" t="str">
         <f>A2&amp;" - "&amp;B2</f>
         <v>P01 - Planning</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="38.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="38.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="24" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D3" s="20">
         <v>2</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="30" t="str">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="str">
         <f>A3&amp;" - "&amp;B3</f>
         <v>P02 - Preparation</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="24" t="s">
+        <v>1798</v>
+      </c>
+      <c r="D4" s="20">
         <v>3</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="E4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="30" t="str">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30" t="str">
         <f>A4&amp;" - "&amp;B4</f>
         <v>P03 - Execution</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="24" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D5" s="20">
         <v>4</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="E5" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="30" t="str">
+      <c r="F5" s="30"/>
+      <c r="G5" s="30" t="str">
         <f>A5&amp;" - "&amp;B5</f>
         <v>P04 - Evaluation</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="34"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="34"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="34"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="37"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.27777777777777801"/>
@@ -12374,24 +12470,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AML13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="1" customWidth="1"/>
-    <col min="5" max="5" width="86.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" style="1" customWidth="1"/>
-    <col min="7" max="1024" width="16.33203125" style="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="74.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="54.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" style="1" customWidth="1"/>
+    <col min="9" max="1026" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>1421</v>
       </c>
@@ -12399,19 +12497,25 @@
         <v>57</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
+        <v>1795</v>
+      </c>
+      <c r="H1" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29" t="s">
         <v>74</v>
       </c>
@@ -12419,20 +12523,24 @@
         <v>75</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>1800</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="20">
+      <c r="E2" s="20">
         <v>1</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="F2" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="30" t="str">
-        <f t="shared" ref="F2:F13" si="0">A2&amp;" - "&amp;B2</f>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30" t="str">
+        <f t="shared" ref="H2:H13" si="0">A2&amp;" - "&amp;B2</f>
         <v>TA01 - Strategic Planning</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="86.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="86.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
         <v>77</v>
       </c>
@@ -12440,20 +12548,24 @@
         <v>78</v>
       </c>
       <c r="C3" s="24" t="s">
+        <v>1801</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="20">
+      <c r="E3" s="20">
         <v>2</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="30" t="str">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA02 - Objective Planning</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>80</v>
       </c>
@@ -12461,20 +12573,24 @@
         <v>81</v>
       </c>
       <c r="C4" s="24" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="20">
+      <c r="E4" s="20">
         <v>3</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="F4" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="30" t="str">
+      <c r="G4" s="30"/>
+      <c r="H4" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA03 - Develop People</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>83</v>
       </c>
@@ -12482,20 +12598,24 @@
         <v>84</v>
       </c>
       <c r="C5" s="24" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="20">
+      <c r="E5" s="20">
         <v>4</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="F5" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="30" t="str">
+      <c r="G5" s="30"/>
+      <c r="H5" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA04 - Develop Networks</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
         <v>86</v>
       </c>
@@ -12503,20 +12623,24 @@
         <v>87</v>
       </c>
       <c r="C6" s="24" t="s">
+        <v>1804</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="20">
+      <c r="E6" s="20">
         <v>5</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="F6" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="30" t="str">
+      <c r="G6" s="30"/>
+      <c r="H6" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA05 - Microtargeting</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>89</v>
       </c>
@@ -12524,20 +12648,24 @@
         <v>90</v>
       </c>
       <c r="C7" s="24" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="20">
+      <c r="E7" s="20">
         <v>6</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="F7" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="30" t="str">
+      <c r="G7" s="30"/>
+      <c r="H7" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA06 - Develop Content</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>92</v>
       </c>
@@ -12545,20 +12673,24 @@
         <v>93</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="20">
+      <c r="E8" s="20">
         <v>7</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="F8" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="30" t="str">
+      <c r="G8" s="30"/>
+      <c r="H8" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA07 - Channel Selection</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>95</v>
       </c>
@@ -12566,99 +12698,111 @@
         <v>96</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="20">
+      <c r="E9" s="20">
         <v>8</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="F9" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="30" t="str">
+      <c r="G9" s="30"/>
+      <c r="H9" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA08 - Pump Priming</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="20">
+      <c r="E10" s="20">
         <v>9</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="F10" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="30" t="str">
+      <c r="G10" s="30"/>
+      <c r="H10" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA09 - Exposure</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>101</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="20">
+      <c r="E11" s="20">
         <v>10</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="30" t="str">
+      <c r="G11" s="30"/>
+      <c r="H11" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA10 - Go Physical</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>104</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="20">
+      <c r="E12" s="20">
         <v>11</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="F12" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="F12" s="30" t="str">
+      <c r="G12" s="30"/>
+      <c r="H12" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA11 - Persistence</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="29" t="s">
         <v>107</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="20">
+      <c r="E13" s="20">
         <v>12</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="F13" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="30" t="str">
+      <c r="G13" s="30"/>
+      <c r="H13" s="30" t="str">
         <f t="shared" si="0"/>
         <v>TA12 - Measure Effectiveness</v>
       </c>
@@ -12677,24 +12821,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ65"/>
+  <dimension ref="A1:AML65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7" style="93" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="93" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="93" customWidth="1"/>
-    <col min="4" max="4" width="92.33203125" style="93" customWidth="1"/>
-    <col min="5" max="5" width="35.83203125" style="93" customWidth="1"/>
-    <col min="6" max="1024" width="16.33203125" style="93"/>
-    <col min="1025" max="16384" width="16.33203125" style="94"/>
+    <col min="2" max="3" width="23.6640625" style="93" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="93" customWidth="1"/>
+    <col min="5" max="6" width="92.33203125" style="93" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" style="93" customWidth="1"/>
+    <col min="8" max="1026" width="16.33203125" style="93"/>
+    <col min="1027" max="16384" width="16.33203125" style="94"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>1421</v>
       </c>
@@ -12702,1163 +12846,1297 @@
         <v>57</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
+        <v>1795</v>
+      </c>
+      <c r="G1" s="40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29" t="s">
         <v>111</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="86"/>
+      <c r="D2" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="89" t="s">
+      <c r="E2" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="95" t="str">
-        <f t="shared" ref="E2:E33" si="0">A2&amp;" - "&amp;B2</f>
+      <c r="F2" s="102"/>
+      <c r="G2" s="95" t="str">
+        <f t="shared" ref="G2:G33" si="0">A2&amp;" - "&amp;B2</f>
         <v>T0001 - 5Ds (dismiss, distort, distract, dismay, divide)</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
         <v>114</v>
       </c>
       <c r="B3" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="89" t="s">
+      <c r="E3" s="89" t="s">
         <v>1539</v>
       </c>
-      <c r="E3" s="95" t="str">
+      <c r="F3" s="102"/>
+      <c r="G3" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0002 - Facilitate State Propaganda</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="E4" s="89" t="s">
         <v>1540</v>
       </c>
-      <c r="E4" s="95" t="str">
+      <c r="F4" s="102"/>
+      <c r="G4" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0003 - Leverage Existing Narratives</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="124" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="124" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>118</v>
       </c>
       <c r="B5" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="86"/>
+      <c r="D5" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="E5" s="89" t="s">
         <v>1541</v>
       </c>
-      <c r="E5" s="95" t="str">
+      <c r="F5" s="102"/>
+      <c r="G5" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0004 - Competing Narratives</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="E6" s="89" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="95" t="str">
+      <c r="F6" s="102"/>
+      <c r="G6" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0005 - Center of Gravity Analysis</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="98" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="98" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>123</v>
       </c>
       <c r="B7" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="89" t="s">
+      <c r="E7" s="89" t="s">
         <v>1542</v>
       </c>
-      <c r="E7" s="95" t="str">
+      <c r="F7" s="102"/>
+      <c r="G7" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0006 - Create Master Narratives</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="85" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="85" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="86"/>
+      <c r="D8" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="89" t="s">
+      <c r="E8" s="89" t="s">
         <v>1543</v>
       </c>
-      <c r="E8" s="95" t="str">
+      <c r="F8" s="102"/>
+      <c r="G8" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0007 - Create fake Social Media Profiles / Pages / Groups</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="86"/>
+      <c r="D9" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="89" t="s">
+      <c r="E9" s="89" t="s">
         <v>1544</v>
       </c>
-      <c r="E9" s="95" t="str">
+      <c r="F9" s="102"/>
+      <c r="G9" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0008 - Create fake or imposter news sites</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>129</v>
       </c>
       <c r="B10" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="86"/>
+      <c r="D10" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="89" t="s">
+      <c r="E10" s="89" t="s">
         <v>1545</v>
       </c>
-      <c r="E10" s="95" t="str">
+      <c r="F10" s="102"/>
+      <c r="G10" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0009 - Create fake experts</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="109" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="109" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>131</v>
       </c>
       <c r="B11" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="86"/>
+      <c r="D11" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="89" t="s">
+      <c r="E11" s="89" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="95" t="str">
+      <c r="F11" s="102"/>
+      <c r="G11" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0010 - Cultivate ignorant agents</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>134</v>
       </c>
       <c r="B12" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="89" t="s">
+      <c r="E12" s="89" t="s">
         <v>1546</v>
       </c>
-      <c r="E12" s="95" t="str">
+      <c r="F12" s="102"/>
+      <c r="G12" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0011 - Hijack legitimate account</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="29" t="s">
         <v>136</v>
       </c>
       <c r="B13" s="86" t="s">
         <v>137</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="86"/>
+      <c r="D13" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="E13" s="89" t="s">
         <v>1547</v>
       </c>
-      <c r="E13" s="95" t="str">
+      <c r="F13" s="102"/>
+      <c r="G13" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0012 - Use concealment</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
         <v>138</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="86"/>
+      <c r="D14" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="E14" s="86" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="95" t="str">
+      <c r="F14" s="95"/>
+      <c r="G14" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0013 - Create fake websites</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
         <v>141</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="86"/>
+      <c r="D15" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="E15" s="89" t="s">
         <v>1548</v>
       </c>
-      <c r="E15" s="95" t="str">
+      <c r="F15" s="102"/>
+      <c r="G15" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0014 - Create funding campaigns</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="122" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
         <v>143</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="86"/>
+      <c r="D16" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="89" t="s">
+      <c r="E16" s="89" t="s">
         <v>1549</v>
       </c>
-      <c r="E16" s="95" t="str">
+      <c r="F16" s="102"/>
+      <c r="G16" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0015 - Create hashtag</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="29" t="s">
         <v>145</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="86"/>
+      <c r="D17" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="89" t="s">
+      <c r="E17" s="89" t="s">
         <v>1550</v>
       </c>
-      <c r="E17" s="95" t="str">
+      <c r="F17" s="102"/>
+      <c r="G17" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0016 - Clickbait</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="29" t="s">
         <v>147</v>
       </c>
       <c r="B18" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="86"/>
+      <c r="D18" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="89" t="s">
+      <c r="E18" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="95" t="str">
+      <c r="F18" s="102"/>
+      <c r="G18" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0017 - Promote online funding</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="29" t="s">
         <v>150</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="86" t="s">
+      <c r="C19" s="86"/>
+      <c r="D19" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="E19" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="95" t="str">
+      <c r="F19" s="102"/>
+      <c r="G19" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0018 - Paid targeted ads</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="29" t="s">
         <v>153</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="86"/>
+      <c r="D20" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="89" t="s">
+      <c r="E20" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="E20" s="95" t="str">
+      <c r="F20" s="102"/>
+      <c r="G20" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0019 - Generate information pollution</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="29" t="s">
         <v>156</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="86"/>
+      <c r="D21" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="E21" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="E21" s="95" t="str">
+      <c r="F21" s="102"/>
+      <c r="G21" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0020 - Trial content</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="74" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="29" t="s">
         <v>159</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="86"/>
+      <c r="D22" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="90" t="s">
+      <c r="E22" s="90" t="s">
         <v>161</v>
       </c>
-      <c r="E22" s="95" t="str">
+      <c r="F22" s="95"/>
+      <c r="G22" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0021 - Memes</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="61" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="29" t="s">
         <v>162</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>163</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="86"/>
+      <c r="D23" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="91" t="s">
+      <c r="E23" s="91" t="s">
         <v>1551</v>
       </c>
-      <c r="E23" s="95" t="str">
+      <c r="F23" s="95"/>
+      <c r="G23" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0022 - Conspiracy narratives</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="29" t="s">
         <v>164</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>165</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="86" t="s">
+      <c r="E24" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="E24" s="95" t="str">
+      <c r="F24" s="95"/>
+      <c r="G24" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0023 - Distort facts</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="29" t="s">
         <v>167</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="86"/>
+      <c r="D25" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="89" t="s">
+      <c r="E25" s="89" t="s">
         <v>1552</v>
       </c>
-      <c r="E25" s="95" t="str">
+      <c r="F25" s="102"/>
+      <c r="G25" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0024 - Create fake videos and images</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="29" t="s">
         <v>169</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="86"/>
+      <c r="D26" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="89" t="s">
+      <c r="E26" s="89" t="s">
         <v>1553</v>
       </c>
-      <c r="E26" s="95" t="str">
+      <c r="F26" s="102"/>
+      <c r="G26" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0025 - Leak altered documents</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="29" t="s">
         <v>171</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="C27" s="86" t="s">
+      <c r="C27" s="86"/>
+      <c r="D27" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="89" t="s">
+      <c r="E27" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="E27" s="95" t="str">
+      <c r="F27" s="102"/>
+      <c r="G27" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0026 - Create fake research</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="82" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="82" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="29" t="s">
         <v>174</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="86"/>
+      <c r="D28" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="90" t="s">
+      <c r="E28" s="90" t="s">
         <v>176</v>
       </c>
-      <c r="E28" s="95" t="str">
+      <c r="F28" s="95"/>
+      <c r="G28" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0027 - Adapt existing narratives</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="136" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="29" t="s">
         <v>177</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="86"/>
+      <c r="D29" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="E29" s="91" t="s">
         <v>179</v>
       </c>
-      <c r="E29" s="95" t="str">
+      <c r="F29" s="95"/>
+      <c r="G29" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0028 - Create competing narratives</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="29" t="s">
         <v>180</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="86"/>
+      <c r="D30" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="89" t="s">
+      <c r="E30" s="89" t="s">
         <v>1554</v>
       </c>
-      <c r="E30" s="95" t="str">
+      <c r="F30" s="102"/>
+      <c r="G30" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0029 - Manipulate online polls</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="29" t="s">
         <v>182</v>
       </c>
       <c r="B31" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="86"/>
+      <c r="D31" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="86" t="s">
+      <c r="E31" s="86" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="95" t="str">
+      <c r="F31" s="95"/>
+      <c r="G31" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0030 - Backstop personas</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="29" t="s">
         <v>185</v>
       </c>
       <c r="B32" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="86" t="s">
+      <c r="C32" s="86"/>
+      <c r="D32" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="90" t="s">
+      <c r="E32" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="E32" s="95" t="str">
+      <c r="F32" s="95"/>
+      <c r="G32" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0031 - YouTube</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="29" t="s">
         <v>188</v>
       </c>
       <c r="B33" s="86" t="s">
         <v>189</v>
       </c>
-      <c r="C33" s="86" t="s">
+      <c r="C33" s="86"/>
+      <c r="D33" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="95" t="s">
+      <c r="E33" s="95" t="s">
         <v>190</v>
       </c>
-      <c r="E33" s="95" t="str">
+      <c r="F33" s="95"/>
+      <c r="G33" s="95" t="str">
         <f t="shared" si="0"/>
         <v>T0032 - Reddit</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="29" t="s">
         <v>191</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>192</v>
       </c>
-      <c r="C34" s="86" t="s">
+      <c r="C34" s="86"/>
+      <c r="D34" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="95" t="s">
+      <c r="E34" s="95" t="s">
         <v>193</v>
       </c>
-      <c r="E34" s="95" t="str">
-        <f t="shared" ref="E34:E65" si="1">A34&amp;" - "&amp;B34</f>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95" t="str">
+        <f t="shared" ref="G34:G65" si="1">A34&amp;" - "&amp;B34</f>
         <v>T0033 - Instagram</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="29" t="s">
         <v>194</v>
       </c>
       <c r="B35" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="C35" s="86" t="s">
+      <c r="C35" s="86"/>
+      <c r="D35" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="E35" s="95" t="s">
         <v>196</v>
       </c>
-      <c r="E35" s="95" t="str">
+      <c r="F35" s="95"/>
+      <c r="G35" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0034 - LinkedIn</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="29" t="s">
         <v>197</v>
       </c>
       <c r="B36" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="86"/>
+      <c r="D36" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="95" t="s">
+      <c r="E36" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="E36" s="95" t="str">
+      <c r="F36" s="95"/>
+      <c r="G36" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0035 - Pinterest</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="29" t="s">
         <v>200</v>
       </c>
       <c r="B37" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="C37" s="86" t="s">
+      <c r="C37" s="86"/>
+      <c r="D37" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="95" t="s">
+      <c r="E37" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="E37" s="95" t="str">
+      <c r="F37" s="95"/>
+      <c r="G37" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0036 - WhatsApp</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="29" t="s">
         <v>203</v>
       </c>
       <c r="B38" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="C38" s="86" t="s">
+      <c r="C38" s="86"/>
+      <c r="D38" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="95" t="s">
+      <c r="E38" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="E38" s="95" t="str">
+      <c r="F38" s="95"/>
+      <c r="G38" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0037 - Facebook</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="29" t="s">
         <v>206</v>
       </c>
       <c r="B39" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="C39" s="86" t="s">
+      <c r="C39" s="86"/>
+      <c r="D39" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D39" s="91" t="s">
+      <c r="E39" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="E39" s="95" t="str">
+      <c r="F39" s="95"/>
+      <c r="G39" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0038 - Twitter</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="29" t="s">
         <v>209</v>
       </c>
       <c r="B40" s="86" t="s">
         <v>210</v>
       </c>
-      <c r="C40" s="86" t="s">
+      <c r="C40" s="86"/>
+      <c r="D40" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D40" s="89" t="s">
+      <c r="E40" s="89" t="s">
         <v>211</v>
       </c>
-      <c r="E40" s="95" t="str">
+      <c r="F40" s="102"/>
+      <c r="G40" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0039 - Bait legitimate influencers</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="29" t="s">
         <v>212</v>
       </c>
       <c r="B41" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="C41" s="86" t="s">
+      <c r="C41" s="86"/>
+      <c r="D41" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="89" t="s">
+      <c r="E41" s="89" t="s">
         <v>214</v>
       </c>
-      <c r="E41" s="95" t="str">
+      <c r="F41" s="102"/>
+      <c r="G41" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0040 - Demand unsurmountable proof</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="44.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7" ht="44.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="29" t="s">
         <v>215</v>
       </c>
       <c r="B42" s="86" t="s">
         <v>216</v>
       </c>
-      <c r="C42" s="86" t="s">
+      <c r="C42" s="86"/>
+      <c r="D42" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="89" t="s">
+      <c r="E42" s="89" t="s">
         <v>217</v>
       </c>
-      <c r="E42" s="95" t="str">
+      <c r="F42" s="102"/>
+      <c r="G42" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0041 - Deny involvement</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="141" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7" ht="141" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="29" t="s">
         <v>218</v>
       </c>
       <c r="B43" s="86" t="s">
         <v>219</v>
       </c>
-      <c r="C43" s="86" t="s">
+      <c r="C43" s="86"/>
+      <c r="D43" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="89" t="s">
+      <c r="E43" s="89" t="s">
         <v>1568</v>
       </c>
-      <c r="E43" s="95" t="str">
+      <c r="F43" s="102"/>
+      <c r="G43" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0042 - Kernel of Truth</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="46" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="29" t="s">
         <v>220</v>
       </c>
       <c r="B44" s="86" t="s">
         <v>221</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="86"/>
+      <c r="D44" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="86" t="s">
+      <c r="E44" s="86" t="s">
         <v>222</v>
       </c>
-      <c r="E44" s="95" t="str">
+      <c r="F44" s="95"/>
+      <c r="G44" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0043 - Use SMS/ WhatsApp/ Chat apps</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="29" t="s">
         <v>223</v>
       </c>
       <c r="B45" s="86" t="s">
         <v>224</v>
       </c>
-      <c r="C45" s="86" t="s">
+      <c r="C45" s="86"/>
+      <c r="D45" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="89" t="s">
+      <c r="E45" s="89" t="s">
         <v>1555</v>
       </c>
-      <c r="E45" s="95" t="str">
+      <c r="F45" s="102"/>
+      <c r="G45" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0044 - Seed distortions</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7" ht="26.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="29" t="s">
         <v>225</v>
       </c>
       <c r="B46" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="C46" s="86" t="s">
+      <c r="C46" s="86"/>
+      <c r="D46" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="86" t="s">
+      <c r="E46" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="E46" s="95" t="str">
+      <c r="F46" s="95"/>
+      <c r="G46" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0045 - Use fake experts</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7" ht="29.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="29" t="s">
         <v>228</v>
       </c>
       <c r="B47" s="86" t="s">
         <v>229</v>
       </c>
-      <c r="C47" s="86" t="s">
+      <c r="C47" s="86"/>
+      <c r="D47" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="89" t="s">
+      <c r="E47" s="89" t="s">
         <v>230</v>
       </c>
-      <c r="E47" s="95" t="str">
+      <c r="F47" s="102"/>
+      <c r="G47" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0046 - Search Engine Optimization</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="29" t="s">
         <v>231</v>
       </c>
       <c r="B48" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="C48" s="86" t="s">
+      <c r="C48" s="86"/>
+      <c r="D48" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D48" s="86" t="s">
+      <c r="E48" s="86" t="s">
         <v>1556</v>
       </c>
-      <c r="E48" s="95" t="str">
+      <c r="F48" s="95"/>
+      <c r="G48" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0047 - Muzzle social media as a political force</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="29" t="s">
         <v>233</v>
       </c>
       <c r="B49" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="C49" s="86" t="s">
+      <c r="C49" s="86"/>
+      <c r="D49" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D49" s="89" t="s">
+      <c r="E49" s="89" t="s">
         <v>1557</v>
       </c>
-      <c r="E49" s="95" t="str">
+      <c r="F49" s="102"/>
+      <c r="G49" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0048 - Cow online opinion leaders</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="29" t="s">
         <v>235</v>
       </c>
       <c r="B50" s="86" t="s">
         <v>236</v>
       </c>
-      <c r="C50" s="86" t="s">
+      <c r="C50" s="86"/>
+      <c r="D50" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="89" t="s">
+      <c r="E50" s="89" t="s">
         <v>1558</v>
       </c>
-      <c r="E50" s="95" t="str">
+      <c r="F50" s="102"/>
+      <c r="G50" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0049 - Flooding</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="29" t="s">
         <v>237</v>
       </c>
       <c r="B51" s="86" t="s">
         <v>238</v>
       </c>
-      <c r="C51" s="86" t="s">
+      <c r="C51" s="86"/>
+      <c r="D51" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="89" t="s">
+      <c r="E51" s="89" t="s">
         <v>1559</v>
       </c>
-      <c r="E51" s="95" t="str">
+      <c r="F51" s="102"/>
+      <c r="G51" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0050 - Cheerleading domestic social media ops</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="29" t="s">
         <v>239</v>
       </c>
       <c r="B52" s="86" t="s">
         <v>240</v>
       </c>
-      <c r="C52" s="86" t="s">
+      <c r="C52" s="86"/>
+      <c r="D52" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="86" t="s">
+      <c r="E52" s="86" t="s">
         <v>1560</v>
       </c>
-      <c r="E52" s="95" t="str">
+      <c r="F52" s="95"/>
+      <c r="G52" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0051 - Fabricate social media comment</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="29" t="s">
         <v>241</v>
       </c>
       <c r="B53" s="86" t="s">
         <v>242</v>
       </c>
-      <c r="C53" s="86" t="s">
+      <c r="C53" s="86"/>
+      <c r="D53" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D53" s="92" t="s">
+      <c r="E53" s="92" t="s">
         <v>1561</v>
       </c>
-      <c r="E53" s="95" t="str">
+      <c r="F53" s="103"/>
+      <c r="G53" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0052 - Tertiary sites amplify news</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="74.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7" ht="74.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="29" t="s">
         <v>243</v>
       </c>
       <c r="B54" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="C54" s="86" t="s">
+      <c r="C54" s="86"/>
+      <c r="D54" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D54" s="89" t="s">
+      <c r="E54" s="89" t="s">
         <v>1562</v>
       </c>
-      <c r="E54" s="95" t="str">
+      <c r="F54" s="102"/>
+      <c r="G54" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0053 - Twitter trolls amplify and manipulate</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="74.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7" ht="74.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="29" t="s">
         <v>245</v>
       </c>
       <c r="B55" s="86" t="s">
         <v>246</v>
       </c>
-      <c r="C55" s="86" t="s">
+      <c r="C55" s="86"/>
+      <c r="D55" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="89" t="s">
+      <c r="E55" s="89" t="s">
         <v>1563</v>
       </c>
-      <c r="E55" s="95" t="str">
+      <c r="F55" s="102"/>
+      <c r="G55" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0054 - Twitter bots amplify</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7" ht="29.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="29" t="s">
         <v>247</v>
       </c>
       <c r="B56" s="86" t="s">
         <v>248</v>
       </c>
-      <c r="C56" s="86" t="s">
+      <c r="C56" s="86"/>
+      <c r="D56" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D56" s="89" t="s">
+      <c r="E56" s="89" t="s">
         <v>1564</v>
       </c>
-      <c r="E56" s="95" t="str">
+      <c r="F56" s="102"/>
+      <c r="G56" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0055 - Use hashtag</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="38.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7" ht="38.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="29" t="s">
         <v>249</v>
       </c>
       <c r="B57" s="86" t="s">
         <v>250</v>
       </c>
-      <c r="C57" s="86" t="s">
+      <c r="C57" s="86"/>
+      <c r="D57" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="D57" s="86" t="s">
+      <c r="E57" s="86" t="s">
         <v>1565</v>
       </c>
-      <c r="E57" s="95" t="str">
+      <c r="F57" s="95"/>
+      <c r="G57" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0056 - Dedicated channels disseminate information pollution</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="29" t="s">
         <v>251</v>
       </c>
       <c r="B58" s="86" t="s">
         <v>252</v>
       </c>
-      <c r="C58" s="86" t="s">
+      <c r="C58" s="86"/>
+      <c r="D58" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="89" t="s">
+      <c r="E58" s="89" t="s">
         <v>1566</v>
       </c>
-      <c r="E58" s="95" t="str">
+      <c r="F58" s="102"/>
+      <c r="G58" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0057 - Organise remote rallies and events</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="29" t="s">
         <v>253</v>
       </c>
       <c r="B59" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="C59" s="86" t="s">
+      <c r="C59" s="86"/>
+      <c r="D59" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="D59" s="89" t="s">
+      <c r="E59" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="E59" s="95" t="str">
+      <c r="F59" s="102"/>
+      <c r="G59" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0058 - Legacy web content</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="61" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="29" t="s">
         <v>256</v>
       </c>
       <c r="B60" s="86" t="s">
         <v>257</v>
       </c>
-      <c r="C60" s="86" t="s">
+      <c r="C60" s="86"/>
+      <c r="D60" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="D60" s="86" t="s">
+      <c r="E60" s="86" t="s">
         <v>1567</v>
       </c>
-      <c r="E60" s="95" t="str">
+      <c r="F60" s="95"/>
+      <c r="G60" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0059 - Play the long game</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="29" t="s">
         <v>258</v>
       </c>
       <c r="B61" s="86" t="s">
         <v>259</v>
       </c>
-      <c r="C61" s="86" t="s">
+      <c r="C61" s="86"/>
+      <c r="D61" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="D61" s="86" t="s">
+      <c r="E61" s="86" t="s">
         <v>260</v>
       </c>
-      <c r="E61" s="95" t="str">
+      <c r="F61" s="95"/>
+      <c r="G61" s="95" t="str">
         <f t="shared" si="1"/>
         <v>T0060 - Continue to amplify</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="29" t="s">
         <v>261</v>
       </c>
       <c r="B62" s="89" t="s">
         <v>262</v>
       </c>
-      <c r="C62" s="89" t="s">
+      <c r="C62" s="89"/>
+      <c r="D62" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="D62" s="89" t="s">
+      <c r="E62" s="89" t="s">
         <v>263</v>
       </c>
-      <c r="E62" s="91" t="str">
+      <c r="F62" s="104"/>
+      <c r="G62" s="91" t="str">
         <f t="shared" si="1"/>
         <v>T0061 - Sell merchandising</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="29" t="s">
         <v>264</v>
       </c>
       <c r="B63" s="89" t="s">
         <v>265</v>
       </c>
-      <c r="C63" s="89" t="s">
+      <c r="C63" s="89"/>
+      <c r="D63" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="D63" s="89" t="s">
+      <c r="E63" s="89" t="s">
         <v>1485</v>
       </c>
-      <c r="E63" s="86" t="str">
+      <c r="F63" s="89"/>
+      <c r="G63" s="86" t="str">
         <f t="shared" si="1"/>
         <v>T0062 - Behaviour changes</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="29" t="s">
         <v>266</v>
       </c>
       <c r="B64" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="C64" s="89" t="s">
+      <c r="C64" s="89"/>
+      <c r="D64" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="D64" s="89" t="s">
+      <c r="E64" s="89" t="s">
         <v>1486</v>
       </c>
-      <c r="E64" s="86" t="str">
+      <c r="F64" s="89"/>
+      <c r="G64" s="86" t="str">
         <f t="shared" si="1"/>
         <v>T0063 - Message reach</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="29" t="s">
         <v>268</v>
       </c>
       <c r="B65" s="89" t="s">
         <v>269</v>
       </c>
-      <c r="C65" s="89" t="s">
+      <c r="C65" s="89"/>
+      <c r="D65" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="D65" s="89" t="s">
+      <c r="E65" s="89" t="s">
         <v>1487</v>
       </c>
-      <c r="E65" s="86" t="str">
+      <c r="F65" s="89"/>
+      <c r="G65" s="86" t="str">
         <f t="shared" si="1"/>
         <v>T0064 - Social media engagement</v>
       </c>
@@ -13874,21 +14152,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10227DA0-E6E4-A64F-BDF9-1BDD39A1750F}">
-  <dimension ref="A1:AMI4"/>
+  <dimension ref="A1:AMK4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1025" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>1421</v>
       </c>
@@ -13896,13 +14174,17 @@
         <v>57</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -14920,48 +15202,50 @@
       <c r="AMG1" s="1"/>
       <c r="AMH1" s="1"/>
       <c r="AMI1" s="1"/>
-    </row>
-    <row r="2" spans="1:1023" ht="14" x14ac:dyDescent="0.15">
+      <c r="AMJ1" s="1"/>
+      <c r="AMK1" s="1"/>
+    </row>
+    <row r="2" spans="1:1025" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="94" t="s">
         <v>1690</v>
       </c>
       <c r="B2" t="s">
         <v>1403</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1406</v>
       </c>
-      <c r="D2" t="str">
+      <c r="F2" t="str">
         <f>A2&amp;" - "&amp;B2</f>
         <v>FW01 - AMITT Red</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1025" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="94" t="s">
         <v>1691</v>
       </c>
       <c r="B3" t="s">
         <v>1404</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1407</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D4" si="0">A3&amp;" - "&amp;B3</f>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F4" si="0">A3&amp;" - "&amp;B3</f>
         <v>FW02 - AMITT Blue</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1025" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="94" t="s">
         <v>1692</v>
       </c>
       <c r="B4" t="s">
         <v>1405</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1408</v>
       </c>
-      <c r="D4" t="str">
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>FW03 - AMITT Green</v>
       </c>
@@ -14976,24 +15260,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK43"/>
+  <dimension ref="A1:AMM43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="1"/>
-    <col min="2" max="2" width="33.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1"/>
-    <col min="4" max="4" width="34.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
-    <col min="7" max="1025" width="16.33203125" style="1"/>
+    <col min="2" max="3" width="33.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="1"/>
+    <col min="5" max="6" width="34.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" style="1" customWidth="1"/>
+    <col min="9" max="1027" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>1421</v>
       </c>
@@ -15001,814 +15285,986 @@
         <v>57</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
+        <v>1795</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>1402</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29" t="s">
         <v>270</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>271</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>1690</v>
       </c>
-      <c r="F2" s="24" t="str">
-        <f t="shared" ref="F2:F43" si="0">A2&amp;" - "&amp;B2</f>
+      <c r="H2" s="24" t="str">
+        <f t="shared" ref="H2:H43" si="0">A2&amp;" - "&amp;B2</f>
         <v>TK0001 - Goal setting</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
         <v>273</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>274</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="20" t="s">
+        <v>1808</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F3" s="24" t="str">
+      <c r="H3" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0002 - Population research / audience analysis (centre of gravity)</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>275</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="20" t="s">
+        <v>1809</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F4" s="24" t="str">
+      <c r="H4" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0003 - Campaign design (objective design)</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>277</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="20" t="s">
+        <v>1810</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F5" s="24" t="str">
+      <c r="H5" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0004 - Identify target subgroups</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
         <v>279</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F6" s="24" t="str">
+      <c r="H6" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0005 - Analyse subgroups</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>281</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F7" s="24" t="str">
+      <c r="H7" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0006 - create master narratives</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>283</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F8" s="24" t="str">
+      <c r="H8" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0007 - Decide on techniques (4Ds etc)</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>285</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="72" t="s">
+      <c r="E9" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F9" s="24" t="str">
+      <c r="H9" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0008 - Create subnarratives</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>287</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F10" s="24" t="str">
+      <c r="H10" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0009 - 4chan/8chan coordinating content</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>289</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F11" s="24" t="str">
+      <c r="H11" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0010 - Create personas</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>291</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="72" t="s">
+      <c r="E12" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F12" s="24" t="str">
+      <c r="H12" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0011 - Recruit contractors</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="29" t="s">
         <v>293</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F13" s="24" t="str">
+      <c r="H13" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0012 - Recruit partisans</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
         <v>295</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F14" s="24" t="str">
+      <c r="H14" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0013 - find influencers</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
         <v>297</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="72" t="s">
+      <c r="E15" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F15" s="24" t="str">
+      <c r="H15" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0014 - Network building</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
         <v>299</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="72" t="s">
+      <c r="E16" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F16" s="24" t="str">
+      <c r="H16" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0015 - Network infiltration</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="29" t="s">
         <v>301</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="72" t="s">
+      <c r="E17" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F17" s="24" t="str">
+      <c r="H17" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0016 - identify targets - susceptible audience members in networks</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="29" t="s">
         <v>303</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F18" s="24" t="str">
+      <c r="H18" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0017 - content creation</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="29" t="s">
         <v>305</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="72" t="s">
+      <c r="E19" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F19" s="24" t="str">
+      <c r="H19" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0018 - content appropriation</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="29" t="s">
         <v>307</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="72" t="s">
+      <c r="E20" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F20" s="24" t="str">
+      <c r="H20" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0019 - anchor trust / credibility</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="29" t="s">
         <v>309</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>310</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="72" t="s">
+      <c r="E21" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F21" s="24" t="str">
+      <c r="H21" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0020 - insert themes</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="29" t="s">
         <v>311</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="72" t="s">
+      <c r="E22" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F22" s="24" t="str">
+      <c r="H22" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0021 - deamplification (suppression, censoring)</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="29" t="s">
         <v>313</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="72" t="s">
+      <c r="E23" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F23" s="24" t="str">
+      <c r="H23" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0022 - amplification</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="29" t="s">
         <v>315</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="72" t="s">
+      <c r="E24" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F24" s="24" t="str">
+      <c r="H24" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0023 - retention</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="29" t="s">
         <v>317</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="24"/>
+      <c r="D25" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="72" t="s">
+      <c r="E25" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F25" s="24" t="str">
+      <c r="H25" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0024 - customer relationship</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="29" t="s">
         <v>319</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="24"/>
+      <c r="D26" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F26" s="24" t="str">
+      <c r="H26" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0025 - advocacy/ zealotry</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="29" t="s">
         <v>321</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="24"/>
+      <c r="D27" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F27" s="24" t="str">
+      <c r="H27" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0026 - conversion</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="29" t="s">
         <v>323</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="24"/>
+      <c r="D28" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F28" s="24" t="str">
+      <c r="H28" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0027 - keep recruiting/prospecting</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="29" t="s">
         <v>325</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="24"/>
+      <c r="D29" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F29" s="24" t="str">
+      <c r="H29" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0028 - evaluation</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="29" t="s">
         <v>327</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="24"/>
+      <c r="D30" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="72" t="s">
+      <c r="E30" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="F30" s="20"/>
+      <c r="G30" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F30" s="24" t="str">
+      <c r="H30" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0029 - post-mortem</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="29" t="s">
         <v>329</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="24"/>
+      <c r="D31" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="72" t="s">
+      <c r="E31" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="72" t="s">
         <v>1690</v>
       </c>
-      <c r="F31" s="24" t="str">
+      <c r="H31" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0030 - after-action analysis</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="29" t="s">
         <v>1409</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="F32" s="105"/>
+      <c r="G32" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F32" s="24" t="str">
+      <c r="H32" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0031 - OPSEC for TA01</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="29" t="s">
         <v>1410</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="24"/>
+      <c r="D33" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="F33" s="35"/>
+      <c r="G33" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F33" s="24" t="str">
+      <c r="H33" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0032 - OPSEC for TA02</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="29" t="s">
         <v>1411</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>333</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="24"/>
+      <c r="D34" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="F34" s="35"/>
+      <c r="G34" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F34" s="24" t="str">
+      <c r="H34" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0033 - OPSEC for TA03</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="29" t="s">
         <v>1412</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>334</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="24"/>
+      <c r="D35" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="F35" s="35"/>
+      <c r="G35" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F35" s="24" t="str">
+      <c r="H35" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0034 - OPSEC for TA04</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="29" t="s">
         <v>1413</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>335</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="24"/>
+      <c r="D36" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="F36" s="35"/>
+      <c r="G36" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F36" s="24" t="str">
+      <c r="H36" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0035 - OPSEC for TA05</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="29" t="s">
         <v>1414</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>336</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="24"/>
+      <c r="D37" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="F37" s="35"/>
+      <c r="G37" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F37" s="24" t="str">
+      <c r="H37" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0036 - OPSEC for TA06</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="29" t="s">
         <v>1415</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="24"/>
+      <c r="D38" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="F38" s="35"/>
+      <c r="G38" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F38" s="24" t="str">
+      <c r="H38" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0037 - OPSEC for TA07</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="29" t="s">
         <v>1416</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="24"/>
+      <c r="D39" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="F39" s="35"/>
+      <c r="G39" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F39" s="24" t="str">
+      <c r="H39" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0038 - OPSEC for TA08</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="29" t="s">
         <v>1417</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="24"/>
+      <c r="D40" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="F40" s="35"/>
+      <c r="G40" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F40" s="24" t="str">
+      <c r="H40" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0039 - OPSEC for TA09</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="29" t="s">
         <v>1418</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>340</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="24"/>
+      <c r="D41" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="F41" s="35"/>
+      <c r="G41" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F41" s="24" t="str">
+      <c r="H41" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0040 - OPSEC for TA10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="29" t="s">
         <v>1419</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="24"/>
+      <c r="D42" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="F42" s="35"/>
+      <c r="G42" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F42" s="24" t="str">
+      <c r="H42" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0041 - OPSEC for TA11</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="29" t="s">
         <v>1420</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="F43" s="35"/>
+      <c r="G43" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="F43" s="24" t="str">
+      <c r="H43" s="24" t="str">
         <f t="shared" si="0"/>
         <v>TK0042 - OPSEC for TA12</v>
       </c>

</xml_diff>